<commit_message>
Modifications to the SDMX modelling
</commit_message>
<xml_diff>
--- a/model/Fishing_location_SDMX_Model.xlsx
+++ b/model/Fishing_location_SDMX_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\rara\RAP\Agriculture\sdd-household-primary-activity-processing\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F002A9-694D-4DED-9205-2E1F0925D396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070ABC9F-92DE-433C-8A9B-5847BCCB9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
   <si>
     <t>Concepts</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Reference area</t>
   </si>
   <si>
-    <t>CL_AREA</t>
-  </si>
-  <si>
     <t>INDICATOR</t>
   </si>
   <si>
@@ -220,25 +217,19 @@
     <t>Othe fishing location</t>
   </si>
   <si>
-    <t>CL_FISHING_INSHORE</t>
-  </si>
-  <si>
-    <t>CL_FISHING_OFFSHORE</t>
-  </si>
-  <si>
-    <t>CL_FISHING_NEARSHORE</t>
-  </si>
-  <si>
     <t>FISHING_OTHER_LOCATION</t>
   </si>
   <si>
-    <t>CL_FISHING_OTHER_LOCATION</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>CL_COM_YESNO</t>
+  </si>
+  <si>
+    <t>CL_COM_GEO_PICT_L123</t>
   </si>
 </sst>
 </file>
@@ -599,7 +590,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +689,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -706,10 +697,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -721,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -729,10 +720,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -744,7 +735,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -752,10 +743,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -767,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -775,13 +766,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -790,21 +781,21 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -816,18 +807,18 @@
         <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -836,21 +827,21 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -859,30 +850,30 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -890,22 +881,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -913,22 +904,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
@@ -936,22 +927,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
@@ -983,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -991,23 +982,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,23 +1053,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,23 +1100,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,23 +1147,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1198,23 +1189,23 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalise the SDMX models for the four new datasets.
</commit_message>
<xml_diff>
--- a/model/Fishing_location_SDMX_Model.xlsx
+++ b/model/Fishing_location_SDMX_Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\rara\RAP\Agriculture\sdd-household-primary-activity-processing\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070ABC9F-92DE-433C-8A9B-5847BCCB9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEAE31E-181E-4341-81A8-1407E5600E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSD" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="71">
   <si>
     <t>Concepts</t>
   </si>
@@ -97,9 +97,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>REF_AREA</t>
-  </si>
-  <si>
     <t>Reference area</t>
   </si>
   <si>
@@ -133,15 +130,9 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>CL_UNIT_MEASURE</t>
-  </si>
-  <si>
     <t>Observation Status</t>
   </si>
   <si>
-    <t>COMMENT</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>CL_OBS_STATUS</t>
-  </si>
-  <si>
     <t>Inshore fishing</t>
   </si>
   <si>
@@ -230,6 +218,42 @@
   </si>
   <si>
     <t>CL_COM_GEO_PICT_L123</t>
+  </si>
+  <si>
+    <t>GEO_PICT</t>
+  </si>
+  <si>
+    <t>CL_COM_UNIT_MEASURE</t>
+  </si>
+  <si>
+    <t>UNIT_MULT</t>
+  </si>
+  <si>
+    <t>Unit multiplier</t>
+  </si>
+  <si>
+    <t>CL_COM_UNIT_MULT</t>
+  </si>
+  <si>
+    <t>CL_COM_OBS_STATUS</t>
+  </si>
+  <si>
+    <t>DATA_SOURCE</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>OBS_COMMENT</t>
+  </si>
+  <si>
+    <t>CONF_STATUS</t>
+  </si>
+  <si>
+    <t>Confidentiality status</t>
+  </si>
+  <si>
+    <t>CL_COM_CONF_STATUS</t>
   </si>
 </sst>
 </file>
@@ -587,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +698,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -689,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -697,10 +721,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -712,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -720,10 +744,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -735,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -743,10 +767,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -758,7 +782,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -766,13 +790,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -781,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -789,13 +813,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -804,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -812,13 +836,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -827,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -835,13 +859,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -850,7 +874,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -858,22 +882,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -881,22 +905,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -904,22 +928,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
@@ -930,21 +954,90 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -974,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,23 +1075,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,23 +1146,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1092,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1100,23 +1193,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,23 +1240,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1189,23 +1282,23 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>